<commit_message>
sscs 10096 update from CCD to make it work with citizens
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherdavidson/Documents/Dev/hmcts/sscs/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAB71FB-F658-D547-9D6D-400FBC639FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E25E57-AF14-5443-BC4F-41109ED1803C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="2840" windowWidth="24460" windowHeight="13900" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,35 +21,36 @@
     <sheet name="CaseTypeTab" sheetId="6" r:id="rId6"/>
     <sheet name="State" sheetId="7" r:id="rId7"/>
     <sheet name="CaseEvent" sheetId="8" r:id="rId8"/>
-    <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId9"/>
-    <sheet name="CaseEventToFields" sheetId="9" r:id="rId10"/>
-    <sheet name="SearchParty" sheetId="21" r:id="rId11"/>
-    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId12"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId13"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId14"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId15"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId16"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId17"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId18"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId19"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId20"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId21"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId22"/>
+    <sheet name="CaseRoles" sheetId="23" r:id="rId9"/>
+    <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId10"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId11"/>
+    <sheet name="SearchParty" sheetId="21" r:id="rId12"/>
+    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId13"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId14"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId15"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId16"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId17"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId18"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId19"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId21"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId23"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$V$110</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">CaseTypeTab!$H$58:$H$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="18">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="19">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="222">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -814,6 +815,9 @@
   </si>
   <si>
     <t>Disabled</t>
+  </si>
+  <si>
+    <t>CaseRoles</t>
   </si>
 </sst>
 </file>
@@ -3004,6 +3008,55 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC9A68F-9D85-C640-9E0E-68D94EA93DB9}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="225"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ229"/>
   <sheetViews>
@@ -5540,7 +5593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FC5E5D-C2A1-6040-955C-8FE864F39FBA}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -5592,7 +5645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -5739,7 +5792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
@@ -7856,7 +7909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -8159,7 +8212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
@@ -8831,7 +8884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
@@ -9302,7 +9355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -9969,7 +10022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:IV35"/>
   <sheetViews>
@@ -10193,7 +10246,188 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="32" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="92.33203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ1015"/>
   <sheetViews>
@@ -24213,188 +24447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="32" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
-    <col min="7" max="7" width="92.33203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
@@ -30441,7 +30494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:IV151"/>
   <sheetViews>
@@ -31491,7 +31544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
@@ -47817,47 +47870,32 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC9A68F-9D85-C640-9E0E-68D94EA93DB9}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4B2DF8-7DAF-784D-BFC2-F63C9A7D3228}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="225"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" t="s">
-        <v>220</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>